<commit_message>
- parsed data from `10.1016/j.apsusc.2025.164997`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2025.xlsx
+++ b/MiscSmallUploads_Nov2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2406C52-506C-5240-A53B-C03081AE0C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02E5C75-F86D-2144-A62A-90DDBC22B382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2360" windowWidth="34560" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7100" windowWidth="34560" windowHeight="12020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="81">
   <si>
     <r>
       <rPr>
@@ -319,6 +319,60 @@
   </si>
   <si>
     <t>hardness HV</t>
+  </si>
+  <si>
+    <t>AAM</t>
+  </si>
+  <si>
+    <t>CrFeNi V0.1 Al0.1</t>
+  </si>
+  <si>
+    <t>CrFeNi V0.1 Al0.5</t>
+  </si>
+  <si>
+    <t>CrFeNi V0.5 Al0.5</t>
+  </si>
+  <si>
+    <t>CrFeNiVAl</t>
+  </si>
+  <si>
+    <t>hardness</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>FCC+BCC</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>BCC+B2</t>
+  </si>
+  <si>
+    <t>corrosion potential</t>
+  </si>
+  <si>
+    <t>3.5 wt% NaCl</t>
+  </si>
+  <si>
+    <t>corrosion current density</t>
+  </si>
+  <si>
+    <t>pitting potential</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A/m^2</t>
+  </si>
+  <si>
+    <t>10.1016/j.apsusc.2025.164997</t>
   </si>
 </sst>
 </file>
@@ -1559,6 +1613,57 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="12" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1618,57 +1723,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2832,8 +2886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M347" sqref="M347"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -2890,19 +2944,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="118" t="s">
+      <c r="D2" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="119"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="123"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="126"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="140"/>
+      <c r="N2" s="143"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -2918,17 +2972,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="130"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="147"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -2969,43 +3023,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="133" t="s">
+      <c r="D5" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="133" t="s">
+      <c r="E5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="133" t="s">
+      <c r="F5" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="133" t="s">
+      <c r="G5" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="134" t="s">
+      <c r="H5" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="133" t="s">
+      <c r="I5" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="133" t="s">
+      <c r="J5" s="150" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="133" t="s">
+      <c r="K5" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="133" t="s">
+      <c r="L5" s="150" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="133" t="s">
+      <c r="M5" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="133" t="s">
+      <c r="N5" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="138" t="s">
+      <c r="O5" s="118" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3021,19 +3075,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="137"/>
-      <c r="K6" s="137"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="O6" s="139"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="152"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="154"/>
+      <c r="K6" s="154"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="119"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3083,7 +3137,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="140"/>
+      <c r="O7" s="120"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3098,35 +3152,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="144" t="s">
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
-      <c r="I8" s="146"/>
-      <c r="J8" s="147"/>
-      <c r="K8" s="147"/>
-      <c r="L8" s="148"/>
-      <c r="M8" s="149" t="s">
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="127"/>
+      <c r="K8" s="127"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="150"/>
+      <c r="N8" s="130"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="151" t="s">
+      <c r="P8" s="131" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="152"/>
-      <c r="R8" s="153"/>
-      <c r="S8" s="153"/>
-      <c r="T8" s="154"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="133"/>
+      <c r="S8" s="133"/>
+      <c r="T8" s="134"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -3190,352 +3244,824 @@
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="30"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
+      <c r="B10" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E10" s="67"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
+      <c r="F10" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="69" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="70"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="72"/>
+      <c r="I10" s="71">
+        <v>298</v>
+      </c>
+      <c r="J10" s="35">
+        <f t="shared" ref="J10:K13" si="0">P10*9807000</f>
+        <v>1814295000</v>
+      </c>
+      <c r="K10" s="35">
+        <f t="shared" si="0"/>
+        <v>61784100</v>
+      </c>
+      <c r="L10" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O10" s="73"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
+      <c r="P10" s="74">
+        <v>185</v>
+      </c>
+      <c r="Q10" s="74">
+        <v>6.3</v>
+      </c>
       <c r="R10" s="74"/>
       <c r="S10" s="73"/>
       <c r="T10" s="73"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="30"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
+      <c r="B11" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E11" s="67"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
+      <c r="F11" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="69" t="s">
+        <v>29</v>
+      </c>
       <c r="H11" s="70"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="72"/>
+      <c r="I11" s="71">
+        <v>298</v>
+      </c>
+      <c r="J11" s="35">
+        <f t="shared" si="0"/>
+        <v>5148675000</v>
+      </c>
+      <c r="K11" s="35">
+        <f t="shared" si="0"/>
+        <v>32363100</v>
+      </c>
+      <c r="L11" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O11" s="37"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
+      <c r="P11" s="38">
+        <v>525</v>
+      </c>
+      <c r="Q11" s="38">
+        <v>3.3</v>
+      </c>
       <c r="R11" s="38"/>
       <c r="S11" s="37"/>
       <c r="T11" s="37"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+      <c r="B12" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E12" s="67"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
+      <c r="F12" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="69" t="s">
+        <v>29</v>
+      </c>
       <c r="H12" s="70"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="72"/>
+      <c r="I12" s="71">
+        <v>298</v>
+      </c>
+      <c r="J12" s="35">
+        <f t="shared" si="0"/>
+        <v>5589990000</v>
+      </c>
+      <c r="K12" s="35">
+        <f t="shared" si="0"/>
+        <v>197120700</v>
+      </c>
+      <c r="L12" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O12" s="37"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
+      <c r="P12" s="38">
+        <v>570</v>
+      </c>
+      <c r="Q12" s="38">
+        <v>20.100000000000001</v>
+      </c>
       <c r="R12" s="38"/>
       <c r="S12" s="37"/>
       <c r="T12" s="37"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E13" s="67"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
+      <c r="F13" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>29</v>
+      </c>
       <c r="H13" s="33"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="72"/>
+      <c r="I13" s="71">
+        <v>298</v>
+      </c>
+      <c r="J13" s="35">
+        <f t="shared" si="0"/>
+        <v>6247059000</v>
+      </c>
+      <c r="K13" s="35">
+        <f t="shared" si="0"/>
+        <v>59822700</v>
+      </c>
+      <c r="L13" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O13" s="37"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
+      <c r="P13" s="38">
+        <v>637</v>
+      </c>
+      <c r="Q13" s="38">
+        <v>6.1</v>
+      </c>
       <c r="R13" s="38"/>
       <c r="S13" s="37"/>
       <c r="T13" s="37"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+      <c r="B14" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E14" s="67"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="72"/>
+      <c r="F14" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="71">
+        <v>298</v>
+      </c>
+      <c r="J14" s="40">
+        <f>-P14*0.001</f>
+        <v>-0.13040000000000002</v>
+      </c>
+      <c r="K14" s="40">
+        <f>-Q14*0.001</f>
+        <v>-3.1000000000000003E-3</v>
+      </c>
+      <c r="L14" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
+      <c r="P14" s="37">
+        <v>130.4</v>
+      </c>
+      <c r="Q14" s="37">
+        <v>3.1</v>
+      </c>
       <c r="R14" s="38"/>
       <c r="S14" s="37"/>
       <c r="T14" s="37"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
+      <c r="B15" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E15" s="67"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="72"/>
+      <c r="F15" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="71">
+        <v>298</v>
+      </c>
+      <c r="J15" s="40">
+        <f t="shared" ref="J15:J17" si="1">-P15*0.001</f>
+        <v>-0.19550000000000001</v>
+      </c>
+      <c r="K15" s="40">
+        <f t="shared" ref="K15:K17" si="2">-Q15*0.001</f>
+        <v>-2.87E-2</v>
+      </c>
+      <c r="L15" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M15" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N15" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
+      <c r="P15" s="37">
+        <v>195.5</v>
+      </c>
+      <c r="Q15" s="37">
+        <v>28.7</v>
+      </c>
       <c r="R15" s="37"/>
       <c r="S15" s="37"/>
       <c r="T15" s="37"/>
     </row>
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
+      <c r="B16" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E16" s="67"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="72"/>
+      <c r="F16" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="71">
+        <v>298</v>
+      </c>
+      <c r="J16" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.26880000000000004</v>
+      </c>
+      <c r="K16" s="40">
+        <f t="shared" si="2"/>
+        <v>-1.2699999999999999E-2</v>
+      </c>
+      <c r="L16" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N16" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
+      <c r="P16" s="37">
+        <v>268.8</v>
+      </c>
+      <c r="Q16" s="37">
+        <v>12.7</v>
+      </c>
       <c r="R16" s="37"/>
       <c r="S16" s="37"/>
       <c r="T16" s="37"/>
     </row>
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="38"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
+      <c r="B17" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E17" s="67"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="72"/>
+      <c r="F17" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="71">
+        <v>298</v>
+      </c>
+      <c r="J17" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.37060000000000004</v>
+      </c>
+      <c r="K17" s="40">
+        <f t="shared" si="2"/>
+        <v>-4.4999999999999998E-2</v>
+      </c>
+      <c r="L17" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N17" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
+      <c r="P17" s="37">
+        <v>370.6</v>
+      </c>
+      <c r="Q17" s="37">
+        <v>45</v>
+      </c>
       <c r="R17" s="37"/>
       <c r="S17" s="37"/>
       <c r="T17" s="37"/>
     </row>
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="38"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
+      <c r="B18" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E18" s="67"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="72"/>
+      <c r="F18" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="71">
+        <v>298</v>
+      </c>
+      <c r="J18" s="71">
+        <f>P18*0.00001</f>
+        <v>1.4600000000000001E-3</v>
+      </c>
+      <c r="K18" s="71">
+        <f>Q18*0.00001</f>
+        <v>1.5000000000000001E-4</v>
+      </c>
+      <c r="L18" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N18" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="39"/>
+      <c r="P18" s="37">
+        <v>146</v>
+      </c>
+      <c r="Q18" s="39">
+        <v>15</v>
+      </c>
       <c r="R18" s="37"/>
       <c r="S18" s="37"/>
       <c r="T18" s="37"/>
     </row>
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="38"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
+      <c r="B19" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E19" s="67"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="71"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="72"/>
+      <c r="F19" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="71">
+        <v>298</v>
+      </c>
+      <c r="J19" s="71">
+        <f t="shared" ref="J19:K21" si="3">P19*0.00001</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="K19" s="71">
+        <f t="shared" si="3"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="L19" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N19" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="39"/>
+      <c r="P19" s="37">
+        <v>160</v>
+      </c>
+      <c r="Q19" s="39">
+        <v>20</v>
+      </c>
       <c r="R19" s="37"/>
       <c r="S19" s="37"/>
       <c r="T19" s="37"/>
     </row>
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="38"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
+      <c r="B20" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E20" s="67"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="72"/>
+      <c r="F20" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="71">
+        <v>298</v>
+      </c>
+      <c r="J20" s="71">
+        <f t="shared" si="3"/>
+        <v>2.8800000000000002E-3</v>
+      </c>
+      <c r="K20" s="71">
+        <f t="shared" si="3"/>
+        <v>3.3000000000000005E-4</v>
+      </c>
+      <c r="L20" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="M20" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N20" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="39"/>
+      <c r="P20" s="37">
+        <v>288</v>
+      </c>
+      <c r="Q20" s="39">
+        <v>33</v>
+      </c>
       <c r="R20" s="37"/>
       <c r="S20" s="37"/>
       <c r="T20" s="37"/>
     </row>
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="38"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
+      <c r="B21" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E21" s="67"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="72"/>
+      <c r="F21" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="71">
+        <v>298</v>
+      </c>
+      <c r="J21" s="71">
+        <f t="shared" si="3"/>
+        <v>2.8900000000000002E-3</v>
+      </c>
+      <c r="K21" s="71">
+        <f t="shared" si="3"/>
+        <v>2.3000000000000001E-4</v>
+      </c>
+      <c r="L21" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="M21" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N21" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="39"/>
+      <c r="P21" s="37">
+        <v>289</v>
+      </c>
+      <c r="Q21" s="39">
+        <v>23</v>
+      </c>
       <c r="R21" s="37"/>
       <c r="S21" s="37"/>
       <c r="T21" s="37"/>
     </row>
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="38"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
+      <c r="B22" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E22" s="67"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="72"/>
+      <c r="F22" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="71">
+        <v>298</v>
+      </c>
+      <c r="J22" s="40">
+        <f>P22*0.001</f>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K22" s="40">
+        <f>Q22*0.001</f>
+        <v>1.4E-2</v>
+      </c>
+      <c r="L22" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M22" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N22" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="39"/>
+      <c r="P22" s="37">
+        <v>976</v>
+      </c>
+      <c r="Q22" s="39">
+        <v>14</v>
+      </c>
       <c r="R22" s="37"/>
       <c r="S22" s="37"/>
       <c r="T22" s="37"/>
     </row>
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
+      <c r="B23" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E23" s="67"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="72"/>
+      <c r="F23" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="71">
+        <v>298</v>
+      </c>
+      <c r="J23" s="40">
+        <f t="shared" ref="J23:J25" si="4">P23*0.001</f>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K23" s="40">
+        <f t="shared" ref="K23:K25" si="5">Q23*0.001</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L23" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M23" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N23" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="39"/>
+      <c r="P23" s="37">
+        <v>976</v>
+      </c>
+      <c r="Q23" s="39">
+        <v>5</v>
+      </c>
       <c r="R23" s="37"/>
       <c r="S23" s="37"/>
       <c r="T23" s="37"/>
     </row>
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="30"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
+      <c r="B24" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E24" s="67"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="72"/>
+      <c r="F24" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" s="71">
+        <v>298</v>
+      </c>
+      <c r="J24" s="40">
+        <f t="shared" si="4"/>
+        <v>1.0474000000000001</v>
+      </c>
+      <c r="K24" s="40">
+        <f t="shared" si="5"/>
+        <v>2.3899999999999998E-2</v>
+      </c>
+      <c r="L24" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N24" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="39"/>
+      <c r="P24" s="37">
+        <v>1047.4000000000001</v>
+      </c>
+      <c r="Q24" s="39">
+        <v>23.9</v>
+      </c>
       <c r="R24" s="37"/>
       <c r="S24" s="37"/>
       <c r="T24" s="37"/>
     </row>
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="88"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
+      <c r="B25" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="68" t="s">
+        <v>63</v>
+      </c>
       <c r="E25" s="67"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="72"/>
+      <c r="F25" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" s="71">
+        <v>298</v>
+      </c>
+      <c r="J25" s="40">
+        <f t="shared" si="4"/>
+        <v>0.1008</v>
+      </c>
+      <c r="K25" s="40">
+        <f t="shared" si="5"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="L25" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M25" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N25" s="72" t="s">
+        <v>80</v>
+      </c>
       <c r="O25" s="37"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="39"/>
+      <c r="P25" s="38">
+        <v>100.8</v>
+      </c>
+      <c r="Q25" s="39">
+        <v>47</v>
+      </c>
       <c r="R25" s="37"/>
       <c r="S25" s="37"/>
       <c r="T25" s="37"/>
@@ -23980,11 +24506,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -23999,6 +24520,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.scriptamat.2025.117086`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2025.xlsx
+++ b/MiscSmallUploads_Nov2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00588E10-C5BD-1E40-9065-A49B84FB74DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A11912-DDBD-F448-991D-02E44EA9BDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="115">
   <si>
     <r>
       <rPr>
@@ -433,6 +433,48 @@
   </si>
   <si>
     <t>10.1007/s10854-025-15540-1</t>
+  </si>
+  <si>
+    <t>W5Hf5Ta35V35Nb20</t>
+  </si>
+  <si>
+    <t>W20Ta35V35Ti10</t>
+  </si>
+  <si>
+    <t>W30Zr5Ta20V35Ti10</t>
+  </si>
+  <si>
+    <t>RD1</t>
+  </si>
+  <si>
+    <t>RD2</t>
+  </si>
+  <si>
+    <t>RD3</t>
+  </si>
+  <si>
+    <t>1e-3 strain rate</t>
+  </si>
+  <si>
+    <t>UCS</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>compressive yield stress</t>
+  </si>
+  <si>
+    <t>compressive ductility</t>
+  </si>
+  <si>
+    <t>minimum compressive ductility</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2025.117086</t>
   </si>
 </sst>
 </file>
@@ -1672,6 +1714,57 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="12" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1731,57 +1824,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2945,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="50" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X48" sqref="X48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3003,19 +3045,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="117" t="s">
+      <c r="D2" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="118"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="125"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="139"/>
+      <c r="N2" s="142"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3031,17 +3073,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="126"/>
-      <c r="M3" s="126"/>
-      <c r="N3" s="129"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="145"/>
+      <c r="K3" s="145"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="146"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3082,43 +3124,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="130" t="s">
+      <c r="C5" s="147" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="132" t="s">
+      <c r="D5" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="132" t="s">
+      <c r="E5" s="149" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="132" t="s">
+      <c r="F5" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="132" t="s">
+      <c r="G5" s="149" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="133" t="s">
+      <c r="H5" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="132" t="s">
+      <c r="I5" s="149" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="132" t="s">
+      <c r="J5" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="132" t="s">
+      <c r="K5" s="149" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="132" t="s">
+      <c r="L5" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="132" t="s">
+      <c r="M5" s="149" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="132" t="s">
+      <c r="N5" s="149" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="137" t="s">
+      <c r="O5" s="117" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3134,19 +3176,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="131"/>
-      <c r="M6" s="131"/>
-      <c r="N6" s="131"/>
-      <c r="O6" s="138"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="148"/>
+      <c r="E6" s="148"/>
+      <c r="F6" s="148"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="152"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="118"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3196,7 +3238,7 @@
       <c r="N7" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="139"/>
+      <c r="O7" s="119"/>
       <c r="P7" s="63" t="s">
         <v>62</v>
       </c>
@@ -3211,35 +3253,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="58"/>
-      <c r="B8" s="140" t="s">
+      <c r="B8" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="143" t="s">
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="144"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="146"/>
-      <c r="K8" s="146"/>
-      <c r="L8" s="147"/>
-      <c r="M8" s="148" t="s">
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="127"/>
+      <c r="M8" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="149"/>
+      <c r="N8" s="129"/>
       <c r="O8" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="150" t="s">
+      <c r="P8" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="151"/>
-      <c r="R8" s="152"/>
-      <c r="S8" s="152"/>
-      <c r="T8" s="153"/>
+      <c r="Q8" s="131"/>
+      <c r="R8" s="132"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="133"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="59" t="s">
@@ -5205,20 +5247,42 @@
       <c r="T49" s="37"/>
     </row>
     <row r="50" spans="1:20" ht="18" customHeight="1">
-      <c r="A50" s="30"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
+      <c r="A50" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>109</v>
+      </c>
       <c r="E50" s="30"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="88"/>
+      <c r="F50" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G50" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H50" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I50" s="34">
+        <v>298</v>
+      </c>
+      <c r="J50" s="88">
+        <v>2362000000</v>
+      </c>
       <c r="K50" s="45"/>
-      <c r="L50" s="32"/>
+      <c r="L50" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M50" s="40"/>
-      <c r="N50" s="36"/>
+      <c r="N50" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="O50" s="44"/>
       <c r="P50" s="44"/>
       <c r="Q50" s="39"/>
@@ -5227,20 +5291,42 @@
       <c r="T50" s="37"/>
     </row>
     <row r="51" spans="1:20" ht="18" customHeight="1">
-      <c r="A51" s="30"/>
-      <c r="B51" s="101"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="89"/>
+      <c r="A51" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>109</v>
+      </c>
       <c r="E51" s="89"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="88"/>
+      <c r="F51" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H51" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I51" s="34">
+        <v>298</v>
+      </c>
+      <c r="J51" s="88">
+        <v>2105000000</v>
+      </c>
       <c r="K51" s="47"/>
-      <c r="L51" s="32"/>
+      <c r="L51" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M51" s="40"/>
-      <c r="N51" s="36"/>
+      <c r="N51" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="O51" s="44"/>
       <c r="P51" s="44"/>
       <c r="Q51" s="39"/>
@@ -5249,20 +5335,42 @@
       <c r="T51" s="37"/>
     </row>
     <row r="52" spans="1:20" ht="18" customHeight="1">
-      <c r="A52" s="30"/>
-      <c r="B52" s="103"/>
-      <c r="C52" s="90"/>
-      <c r="D52" s="90"/>
+      <c r="A52" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" s="103" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>109</v>
+      </c>
       <c r="E52" s="90"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="88"/>
+      <c r="F52" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G52" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H52" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I52" s="34">
+        <v>298</v>
+      </c>
+      <c r="J52" s="88">
+        <v>2039000000</v>
+      </c>
       <c r="K52" s="47"/>
-      <c r="L52" s="32"/>
+      <c r="L52" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M52" s="40"/>
-      <c r="N52" s="36"/>
+      <c r="N52" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="O52" s="44"/>
       <c r="P52" s="45"/>
       <c r="Q52" s="39"/>
@@ -5271,20 +5379,42 @@
       <c r="T52" s="37"/>
     </row>
     <row r="53" spans="1:20" ht="18" customHeight="1">
-      <c r="A53" s="30"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
+      <c r="A53" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>109</v>
+      </c>
       <c r="E53" s="30"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="88"/>
+      <c r="F53" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H53" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I53" s="34">
+        <v>298</v>
+      </c>
+      <c r="J53" s="88">
+        <v>1180000000</v>
+      </c>
       <c r="K53" s="47"/>
-      <c r="L53" s="32"/>
+      <c r="L53" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M53" s="40"/>
-      <c r="N53" s="36"/>
+      <c r="N53" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="O53" s="44"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="44"/>
@@ -5293,20 +5423,42 @@
       <c r="T53" s="37"/>
     </row>
     <row r="54" spans="1:20" ht="18" customHeight="1">
-      <c r="A54" s="30"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="A54" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>109</v>
+      </c>
       <c r="E54" s="30"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="88"/>
+      <c r="F54" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="G54" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I54" s="34">
+        <v>298</v>
+      </c>
+      <c r="J54" s="88">
+        <v>45.2</v>
+      </c>
       <c r="K54" s="47"/>
-      <c r="L54" s="32"/>
+      <c r="L54" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="M54" s="40"/>
-      <c r="N54" s="36"/>
+      <c r="N54" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="O54" s="44"/>
       <c r="P54" s="44"/>
       <c r="Q54" s="44"/>
@@ -5315,20 +5467,42 @@
       <c r="T54" s="37"/>
     </row>
     <row r="55" spans="1:20" ht="18" customHeight="1">
-      <c r="A55" s="30"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="88"/>
+      <c r="A55" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" s="89"/>
+      <c r="F55" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H55" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I55" s="34">
+        <v>298</v>
+      </c>
+      <c r="J55" s="88">
+        <v>11.7</v>
+      </c>
       <c r="K55" s="47"/>
-      <c r="L55" s="32"/>
+      <c r="L55" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="M55" s="40"/>
-      <c r="N55" s="36"/>
+      <c r="N55" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="O55" s="44"/>
       <c r="P55" s="44"/>
       <c r="Q55" s="44"/>
@@ -5337,20 +5511,42 @@
       <c r="T55" s="37"/>
     </row>
     <row r="56" spans="1:20" ht="18" customHeight="1">
-      <c r="A56" s="30"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="88"/>
+      <c r="A56" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="103" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="90"/>
+      <c r="F56" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G56" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H56" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I56" s="34">
+        <v>298</v>
+      </c>
+      <c r="J56" s="88">
+        <v>12.7</v>
+      </c>
       <c r="K56" s="47"/>
-      <c r="L56" s="32"/>
+      <c r="L56" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="M56" s="40"/>
-      <c r="N56" s="36"/>
+      <c r="N56" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="O56" s="44"/>
       <c r="P56" s="44"/>
       <c r="Q56" s="44"/>
@@ -25104,11 +25300,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -25123,6 +25314,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.mtcomm.2025.114374`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2025.xlsx
+++ b/MiscSmallUploads_Nov2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A11912-DDBD-F448-991D-02E44EA9BDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A86809-A871-4544-B058-FA887AB8FE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="120">
   <si>
     <r>
       <rPr>
@@ -475,6 +475,21 @@
   </si>
   <si>
     <t>10.1016/j.scriptamat.2025.117086</t>
+  </si>
+  <si>
+    <t>10.1016/j.mtcomm.2025.114374</t>
+  </si>
+  <si>
+    <t>Co10 Cr20 Cu20 Mn20 Nb10 Ni20</t>
+  </si>
+  <si>
+    <t>sintered at 950*C under 50MPa for 10min</t>
+  </si>
+  <si>
+    <t>L12+C14+B2</t>
+  </si>
+  <si>
+    <t>MA+S</t>
   </si>
 </sst>
 </file>
@@ -2987,8 +3002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -5556,21 +5571,44 @@
     </row>
     <row r="57" spans="1:20" ht="18" customHeight="1">
       <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
+      <c r="B57" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H57" s="33"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="88"/>
+      <c r="I57" s="34">
+        <v>298</v>
+      </c>
+      <c r="J57" s="35">
+        <f t="shared" ref="J57" si="7">P57*9807000</f>
+        <v>4344501000</v>
+      </c>
       <c r="K57" s="47"/>
-      <c r="L57" s="32"/>
+      <c r="L57" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M57" s="40"/>
-      <c r="N57" s="36"/>
+      <c r="N57" s="36" t="s">
+        <v>115</v>
+      </c>
       <c r="O57" s="44"/>
-      <c r="P57" s="44"/>
+      <c r="P57" s="44">
+        <v>443</v>
+      </c>
       <c r="Q57" s="44"/>
       <c r="R57" s="44"/>
       <c r="S57" s="37"/>

</xml_diff>

<commit_message>
- parsed an alloy from `10.3390/ma12060926` without properties because they did not seem sufficiently reliable
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2025.xlsx
+++ b/MiscSmallUploads_Nov2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A86809-A871-4544-B058-FA887AB8FE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF981E1E-3F75-1046-8C58-001DBE9F0647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="125">
   <si>
     <r>
       <rPr>
@@ -490,6 +490,21 @@
   </si>
   <si>
     <t>MA+S</t>
+  </si>
+  <si>
+    <t>AlAgCuNiSnTi</t>
+  </si>
+  <si>
+    <t>VAM</t>
+  </si>
+  <si>
+    <t>VAM+H</t>
+  </si>
+  <si>
+    <t>homogenized at 1073K</t>
+  </si>
+  <si>
+    <t>10.3390/ma12060926</t>
   </si>
 </sst>
 </file>
@@ -3002,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -5616,9 +5631,13 @@
     </row>
     <row r="58" spans="1:20" ht="18" customHeight="1">
       <c r="A58" s="30"/>
-      <c r="B58" s="31"/>
+      <c r="B58" s="31" t="s">
+        <v>120</v>
+      </c>
       <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
+      <c r="D58" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E58" s="30"/>
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
@@ -5628,7 +5647,9 @@
       <c r="K58" s="47"/>
       <c r="L58" s="32"/>
       <c r="M58" s="40"/>
-      <c r="N58" s="36"/>
+      <c r="N58" s="36" t="s">
+        <v>124</v>
+      </c>
       <c r="O58" s="44"/>
       <c r="P58" s="44"/>
       <c r="Q58" s="44"/>
@@ -5638,10 +5659,16 @@
     </row>
     <row r="59" spans="1:20" ht="18" customHeight="1">
       <c r="A59" s="30"/>
-      <c r="B59" s="31"/>
+      <c r="B59" s="31" t="s">
+        <v>120</v>
+      </c>
       <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
+      <c r="D59" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>123</v>
+      </c>
       <c r="F59" s="32"/>
       <c r="G59" s="32"/>
       <c r="H59" s="33"/>
@@ -5650,7 +5677,9 @@
       <c r="K59" s="47"/>
       <c r="L59" s="32"/>
       <c r="M59" s="40"/>
-      <c r="N59" s="36"/>
+      <c r="N59" s="36" t="s">
+        <v>124</v>
+      </c>
       <c r="O59" s="44"/>
       <c r="P59" s="44"/>
       <c r="Q59" s="44"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.msea.2025.149514`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2025.xlsx
+++ b/MiscSmallUploads_Nov2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF981E1E-3F75-1046-8C58-001DBE9F0647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA01CB5-E8D3-C54E-8960-B986E2C96C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="132">
   <si>
     <r>
       <rPr>
@@ -505,6 +505,27 @@
   </si>
   <si>
     <t>10.3390/ma12060926</t>
+  </si>
+  <si>
+    <t>HfNbTiZr</t>
+  </si>
+  <si>
+    <t>AAM+CR+HT</t>
+  </si>
+  <si>
+    <t>cold rolled to 90% reduction and "annealed" at 1050*C for 40s</t>
+  </si>
+  <si>
+    <t>tensile yield stress</t>
+  </si>
+  <si>
+    <t>uniform elongation</t>
+  </si>
+  <si>
+    <t>tensile ductility</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2025.149514</t>
   </si>
 </sst>
 </file>
@@ -3017,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -5689,19 +5710,37 @@
     </row>
     <row r="60" spans="1:20" ht="18" customHeight="1">
       <c r="A60" s="30"/>
-      <c r="B60" s="31"/>
+      <c r="B60" s="31" t="s">
+        <v>125</v>
+      </c>
       <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
+      <c r="D60" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H60" s="33"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="88"/>
+      <c r="I60" s="34">
+        <v>298</v>
+      </c>
+      <c r="J60" s="88">
+        <v>780000000</v>
+      </c>
       <c r="K60" s="47"/>
-      <c r="L60" s="32"/>
+      <c r="L60" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M60" s="40"/>
-      <c r="N60" s="36"/>
+      <c r="N60" s="36" t="s">
+        <v>131</v>
+      </c>
       <c r="O60" s="44"/>
       <c r="P60" s="44"/>
       <c r="Q60" s="44"/>
@@ -5711,19 +5750,37 @@
     </row>
     <row r="61" spans="1:20" ht="18" customHeight="1">
       <c r="A61" s="30"/>
-      <c r="B61" s="31"/>
+      <c r="B61" s="31" t="s">
+        <v>125</v>
+      </c>
       <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
+      <c r="D61" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F61" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H61" s="33"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="88"/>
+      <c r="I61" s="34">
+        <v>298</v>
+      </c>
+      <c r="J61" s="88">
+        <v>4</v>
+      </c>
       <c r="K61" s="47"/>
-      <c r="L61" s="32"/>
+      <c r="L61" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="M61" s="40"/>
-      <c r="N61" s="36"/>
+      <c r="N61" s="36" t="s">
+        <v>131</v>
+      </c>
       <c r="O61" s="44"/>
       <c r="P61" s="44"/>
       <c r="Q61" s="44"/>
@@ -5733,19 +5790,37 @@
     </row>
     <row r="62" spans="1:20" ht="18" customHeight="1">
       <c r="A62" s="30"/>
-      <c r="B62" s="31"/>
+      <c r="B62" s="31" t="s">
+        <v>125</v>
+      </c>
       <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
+      <c r="D62" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="G62" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H62" s="33"/>
-      <c r="I62" s="34"/>
-      <c r="J62" s="88"/>
+      <c r="I62" s="34">
+        <v>298</v>
+      </c>
+      <c r="J62" s="88">
+        <v>33.5</v>
+      </c>
       <c r="K62" s="47"/>
-      <c r="L62" s="32"/>
+      <c r="L62" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="M62" s="40"/>
-      <c r="N62" s="36"/>
+      <c r="N62" s="36" t="s">
+        <v>131</v>
+      </c>
       <c r="O62" s="44"/>
       <c r="P62" s="44"/>
       <c r="Q62" s="44"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.jallcom.2024.173656`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2025.xlsx
+++ b/MiscSmallUploads_Nov2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D860534-256B-0B45-AA77-FDA3C34A8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D3CD1B-C21F-E447-931B-BCE45E6EE7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="156">
   <si>
     <r>
       <rPr>
@@ -568,6 +568,36 @@
   </si>
   <si>
     <t>F5a</t>
+  </si>
+  <si>
+    <t>V14Nb19Mo20Ta24W23</t>
+  </si>
+  <si>
+    <t>V5Nb17Mo19Ta34W25</t>
+  </si>
+  <si>
+    <t>V22Nb24Mo24Ta24W10</t>
+  </si>
+  <si>
+    <t>V21Nb18Mo18Ta22W21</t>
+  </si>
+  <si>
+    <t>"equiatomic"</t>
+  </si>
+  <si>
+    <t>dendritic</t>
+  </si>
+  <si>
+    <t>equiaxial</t>
+  </si>
+  <si>
+    <t>BCC+BCC</t>
+  </si>
+  <si>
+    <t>single BCC with strong segregation or dual BCC with nearly identical lattice constants</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2024.173656</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1793,8 +1823,6 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="14" fillId="10" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -3080,8 +3108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N147" sqref="N147"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A107" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N152" sqref="N152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3138,19 +3166,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="134" t="s">
+      <c r="D2" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="135"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="139"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="141"/>
-      <c r="K2" s="141"/>
-      <c r="L2" s="139"/>
-      <c r="M2" s="139"/>
-      <c r="N2" s="142"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="137"/>
+      <c r="N2" s="140"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3166,17 +3194,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="145"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="143"/>
-      <c r="N3" s="146"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="141"/>
+      <c r="N3" s="144"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3217,43 +3245,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="149" t="s">
+      <c r="D5" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="149" t="s">
+      <c r="E5" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="149" t="s">
+      <c r="F5" s="147" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="149" t="s">
+      <c r="G5" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="150" t="s">
+      <c r="H5" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="149" t="s">
+      <c r="I5" s="147" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="149" t="s">
+      <c r="J5" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="149" t="s">
+      <c r="K5" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="149" t="s">
+      <c r="L5" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="149" t="s">
+      <c r="M5" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="149" t="s">
+      <c r="N5" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="117" t="s">
+      <c r="O5" s="115" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3269,19 +3297,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="148"/>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="151"/>
-      <c r="I6" s="152"/>
-      <c r="J6" s="153"/>
-      <c r="K6" s="153"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="118"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="146"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="150"/>
+      <c r="J6" s="151"/>
+      <c r="K6" s="151"/>
+      <c r="L6" s="146"/>
+      <c r="M6" s="146"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="116"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3331,7 +3359,7 @@
       <c r="N7" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="119"/>
+      <c r="O7" s="117"/>
       <c r="P7" s="63" t="s">
         <v>62</v>
       </c>
@@ -3346,35 +3374,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="58"/>
-      <c r="B8" s="120" t="s">
+      <c r="B8" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="123" t="s">
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="128" t="s">
+      <c r="G8" s="122"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="123"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
+      <c r="L8" s="125"/>
+      <c r="M8" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="129"/>
+      <c r="N8" s="127"/>
       <c r="O8" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="130" t="s">
+      <c r="P8" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="132"/>
-      <c r="S8" s="132"/>
-      <c r="T8" s="133"/>
+      <c r="Q8" s="129"/>
+      <c r="R8" s="130"/>
+      <c r="S8" s="130"/>
+      <c r="T8" s="131"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="59" t="s">
@@ -5871,7 +5899,9 @@
       <c r="T62" s="37"/>
     </row>
     <row r="63" spans="1:20" ht="18" customHeight="1">
-      <c r="A63" s="30"/>
+      <c r="A63" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B63" s="31" t="s">
         <v>132</v>
       </c>
@@ -5920,7 +5950,9 @@
       <c r="T63" s="37"/>
     </row>
     <row r="64" spans="1:20" ht="18" customHeight="1">
-      <c r="A64" s="30"/>
+      <c r="A64" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B64" s="31" t="s">
         <v>132</v>
       </c>
@@ -5969,7 +6001,9 @@
       <c r="T64" s="37"/>
     </row>
     <row r="65" spans="1:20" ht="18" customHeight="1">
-      <c r="A65" s="30"/>
+      <c r="A65" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B65" s="31" t="s">
         <v>132</v>
       </c>
@@ -6018,7 +6052,9 @@
       <c r="T65" s="37"/>
     </row>
     <row r="66" spans="1:20" ht="18" customHeight="1">
-      <c r="A66" s="30"/>
+      <c r="A66" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B66" s="31" t="s">
         <v>132</v>
       </c>
@@ -6067,7 +6103,9 @@
       <c r="T66" s="37"/>
     </row>
     <row r="67" spans="1:20" ht="18" customHeight="1">
-      <c r="A67" s="30"/>
+      <c r="A67" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B67" s="31" t="s">
         <v>132</v>
       </c>
@@ -6116,7 +6154,9 @@
       <c r="T67" s="37"/>
     </row>
     <row r="68" spans="1:20" ht="18" customHeight="1">
-      <c r="A68" s="30"/>
+      <c r="A68" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B68" s="31" t="s">
         <v>132</v>
       </c>
@@ -6165,7 +6205,9 @@
       <c r="T68" s="37"/>
     </row>
     <row r="69" spans="1:20" ht="18" customHeight="1">
-      <c r="A69" s="30"/>
+      <c r="A69" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B69" s="31" t="s">
         <v>132</v>
       </c>
@@ -6214,7 +6256,9 @@
       <c r="T69" s="37"/>
     </row>
     <row r="70" spans="1:20" ht="18" customHeight="1">
-      <c r="A70" s="30"/>
+      <c r="A70" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B70" s="31" t="s">
         <v>132</v>
       </c>
@@ -6263,7 +6307,9 @@
       <c r="T70" s="37"/>
     </row>
     <row r="71" spans="1:20" ht="18" customHeight="1">
-      <c r="A71" s="30"/>
+      <c r="A71" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B71" s="31" t="s">
         <v>132</v>
       </c>
@@ -6312,7 +6358,9 @@
       <c r="T71" s="37"/>
     </row>
     <row r="72" spans="1:20" ht="18" customHeight="1">
-      <c r="A72" s="30"/>
+      <c r="A72" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B72" s="31" t="s">
         <v>132</v>
       </c>
@@ -6361,7 +6409,9 @@
       <c r="T72" s="37"/>
     </row>
     <row r="73" spans="1:20" ht="18" customHeight="1">
-      <c r="A73" s="30"/>
+      <c r="A73" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B73" s="31" t="s">
         <v>132</v>
       </c>
@@ -6410,7 +6460,9 @@
       <c r="T73" s="37"/>
     </row>
     <row r="74" spans="1:20" ht="18" customHeight="1">
-      <c r="A74" s="30"/>
+      <c r="A74" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B74" s="31" t="s">
         <v>132</v>
       </c>
@@ -6459,7 +6511,9 @@
       <c r="T74" s="37"/>
     </row>
     <row r="75" spans="1:20" ht="18" customHeight="1">
-      <c r="A75" s="30"/>
+      <c r="A75" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B75" s="31" t="s">
         <v>132</v>
       </c>
@@ -6508,7 +6562,9 @@
       <c r="T75" s="37"/>
     </row>
     <row r="76" spans="1:20" ht="18" customHeight="1">
-      <c r="A76" s="30"/>
+      <c r="A76" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B76" s="31" t="s">
         <v>132</v>
       </c>
@@ -6557,7 +6613,9 @@
       <c r="T76" s="37"/>
     </row>
     <row r="77" spans="1:20" ht="18" customHeight="1">
-      <c r="A77" s="30"/>
+      <c r="A77" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B77" s="31" t="s">
         <v>132</v>
       </c>
@@ -6606,7 +6664,9 @@
       <c r="T77" s="37"/>
     </row>
     <row r="78" spans="1:20" ht="18" customHeight="1">
-      <c r="A78" s="30"/>
+      <c r="A78" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B78" s="31" t="s">
         <v>132</v>
       </c>
@@ -6655,7 +6715,9 @@
       <c r="T78" s="37"/>
     </row>
     <row r="79" spans="1:20" ht="18" customHeight="1">
-      <c r="A79" s="30"/>
+      <c r="A79" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B79" s="31" t="s">
         <v>132</v>
       </c>
@@ -6704,7 +6766,9 @@
       <c r="T79" s="37"/>
     </row>
     <row r="80" spans="1:20" ht="18" customHeight="1">
-      <c r="A80" s="30"/>
+      <c r="A80" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B80" s="31" t="s">
         <v>132</v>
       </c>
@@ -6753,7 +6817,9 @@
       <c r="T80" s="37"/>
     </row>
     <row r="81" spans="1:20" ht="18" customHeight="1">
-      <c r="A81" s="30"/>
+      <c r="A81" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B81" s="31" t="s">
         <v>132</v>
       </c>
@@ -6802,7 +6868,9 @@
       <c r="T81" s="37"/>
     </row>
     <row r="82" spans="1:20" ht="18" customHeight="1">
-      <c r="A82" s="30"/>
+      <c r="A82" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B82" s="31" t="s">
         <v>132</v>
       </c>
@@ -6851,7 +6919,9 @@
       <c r="T82" s="37"/>
     </row>
     <row r="83" spans="1:20" ht="18" customHeight="1">
-      <c r="A83" s="30"/>
+      <c r="A83" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B83" s="31" t="s">
         <v>132</v>
       </c>
@@ -6900,7 +6970,9 @@
       <c r="T83" s="37"/>
     </row>
     <row r="84" spans="1:20" ht="18" customHeight="1">
-      <c r="A84" s="30"/>
+      <c r="A84" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B84" s="31" t="s">
         <v>132</v>
       </c>
@@ -6949,7 +7021,9 @@
       <c r="T84" s="37"/>
     </row>
     <row r="85" spans="1:20" ht="18" customHeight="1">
-      <c r="A85" s="30"/>
+      <c r="A85" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B85" s="31" t="s">
         <v>132</v>
       </c>
@@ -6998,7 +7072,9 @@
       <c r="T85" s="37"/>
     </row>
     <row r="86" spans="1:20" ht="18" customHeight="1">
-      <c r="A86" s="30"/>
+      <c r="A86" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B86" s="31" t="s">
         <v>132</v>
       </c>
@@ -7047,7 +7123,9 @@
       <c r="T86" s="37"/>
     </row>
     <row r="87" spans="1:20" ht="18" customHeight="1">
-      <c r="A87" s="30"/>
+      <c r="A87" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B87" s="31" t="s">
         <v>132</v>
       </c>
@@ -7096,7 +7174,9 @@
       <c r="T87" s="37"/>
     </row>
     <row r="88" spans="1:20" ht="18" customHeight="1">
-      <c r="A88" s="30"/>
+      <c r="A88" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B88" s="31" t="s">
         <v>132</v>
       </c>
@@ -7145,7 +7225,9 @@
       <c r="T88" s="37"/>
     </row>
     <row r="89" spans="1:20" ht="18" customHeight="1">
-      <c r="A89" s="30"/>
+      <c r="A89" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B89" s="31" t="s">
         <v>132</v>
       </c>
@@ -7194,7 +7276,9 @@
       <c r="T89" s="37"/>
     </row>
     <row r="90" spans="1:20" ht="18" customHeight="1">
-      <c r="A90" s="30"/>
+      <c r="A90" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B90" s="31" t="s">
         <v>132</v>
       </c>
@@ -7243,7 +7327,9 @@
       <c r="T90" s="37"/>
     </row>
     <row r="91" spans="1:20" ht="18" customHeight="1">
-      <c r="A91" s="30"/>
+      <c r="A91" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B91" s="31" t="s">
         <v>132</v>
       </c>
@@ -7292,7 +7378,9 @@
       <c r="T91" s="37"/>
     </row>
     <row r="92" spans="1:20" ht="18" customHeight="1">
-      <c r="A92" s="30"/>
+      <c r="A92" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B92" s="31" t="s">
         <v>132</v>
       </c>
@@ -7341,7 +7429,9 @@
       <c r="T92" s="37"/>
     </row>
     <row r="93" spans="1:20" ht="18" customHeight="1">
-      <c r="A93" s="30"/>
+      <c r="A93" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B93" s="31" t="s">
         <v>132</v>
       </c>
@@ -7390,7 +7480,9 @@
       <c r="T93" s="37"/>
     </row>
     <row r="94" spans="1:20" ht="18" customHeight="1">
-      <c r="A94" s="30"/>
+      <c r="A94" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B94" s="31" t="s">
         <v>132</v>
       </c>
@@ -7439,7 +7531,9 @@
       <c r="T94" s="37"/>
     </row>
     <row r="95" spans="1:20" ht="18" customHeight="1">
-      <c r="A95" s="30"/>
+      <c r="A95" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B95" s="31" t="s">
         <v>132</v>
       </c>
@@ -7488,7 +7582,9 @@
       <c r="T95" s="37"/>
     </row>
     <row r="96" spans="1:20" ht="18" customHeight="1">
-      <c r="A96" s="30"/>
+      <c r="A96" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B96" s="31" t="s">
         <v>132</v>
       </c>
@@ -7537,7 +7633,9 @@
       <c r="T96" s="37"/>
     </row>
     <row r="97" spans="1:20" ht="18" customHeight="1">
-      <c r="A97" s="30"/>
+      <c r="A97" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B97" s="31" t="s">
         <v>132</v>
       </c>
@@ -7586,7 +7684,9 @@
       <c r="T97" s="37"/>
     </row>
     <row r="98" spans="1:20" ht="18" customHeight="1">
-      <c r="A98" s="107"/>
+      <c r="A98" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B98" s="31" t="s">
         <v>132</v>
       </c>
@@ -7635,7 +7735,9 @@
       <c r="T98" s="37"/>
     </row>
     <row r="99" spans="1:20" ht="18" customHeight="1">
-      <c r="A99" s="108"/>
+      <c r="A99" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B99" s="31" t="s">
         <v>132</v>
       </c>
@@ -7684,7 +7786,9 @@
       <c r="T99" s="37"/>
     </row>
     <row r="100" spans="1:20" ht="18" customHeight="1">
-      <c r="A100" s="108"/>
+      <c r="A100" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B100" s="31" t="s">
         <v>132</v>
       </c>
@@ -7733,7 +7837,9 @@
       <c r="T100" s="37"/>
     </row>
     <row r="101" spans="1:20" ht="18" customHeight="1">
-      <c r="A101" s="108"/>
+      <c r="A101" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B101" s="31" t="s">
         <v>132</v>
       </c>
@@ -7782,7 +7888,9 @@
       <c r="T101" s="37"/>
     </row>
     <row r="102" spans="1:20" ht="18" customHeight="1">
-      <c r="A102" s="107"/>
+      <c r="A102" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B102" s="31" t="s">
         <v>132</v>
       </c>
@@ -7831,7 +7939,9 @@
       <c r="T102" s="37"/>
     </row>
     <row r="103" spans="1:20" ht="18" customHeight="1">
-      <c r="A103" s="108"/>
+      <c r="A103" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B103" s="31" t="s">
         <v>132</v>
       </c>
@@ -7880,7 +7990,9 @@
       <c r="T103" s="37"/>
     </row>
     <row r="104" spans="1:20" ht="18" customHeight="1">
-      <c r="A104" s="108"/>
+      <c r="A104" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B104" s="31" t="s">
         <v>132</v>
       </c>
@@ -7929,7 +8041,9 @@
       <c r="T104" s="37"/>
     </row>
     <row r="105" spans="1:20" ht="18" customHeight="1">
-      <c r="A105" s="108"/>
+      <c r="A105" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B105" s="31" t="s">
         <v>132</v>
       </c>
@@ -7980,7 +8094,9 @@
       <c r="T105" s="37"/>
     </row>
     <row r="106" spans="1:20" ht="18" customHeight="1">
-      <c r="A106" s="107"/>
+      <c r="A106" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B106" s="31" t="s">
         <v>132</v>
       </c>
@@ -8031,7 +8147,9 @@
       <c r="T106" s="37"/>
     </row>
     <row r="107" spans="1:20" ht="18" customHeight="1">
-      <c r="A107" s="108"/>
+      <c r="A107" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B107" s="31" t="s">
         <v>132</v>
       </c>
@@ -8082,7 +8200,9 @@
       <c r="T107" s="37"/>
     </row>
     <row r="108" spans="1:20" ht="18" customHeight="1">
-      <c r="A108" s="108"/>
+      <c r="A108" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B108" s="31" t="s">
         <v>132</v>
       </c>
@@ -8133,7 +8253,9 @@
       <c r="T108" s="37"/>
     </row>
     <row r="109" spans="1:20" ht="18" customHeight="1">
-      <c r="A109" s="108"/>
+      <c r="A109" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B109" s="31" t="s">
         <v>132</v>
       </c>
@@ -8184,7 +8306,9 @@
       <c r="T109" s="37"/>
     </row>
     <row r="110" spans="1:20" ht="18" customHeight="1">
-      <c r="A110" s="107"/>
+      <c r="A110" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B110" s="31" t="s">
         <v>132</v>
       </c>
@@ -8235,7 +8359,9 @@
       <c r="T110" s="37"/>
     </row>
     <row r="111" spans="1:20" ht="18" customHeight="1">
-      <c r="A111" s="108"/>
+      <c r="A111" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B111" s="31" t="s">
         <v>132</v>
       </c>
@@ -8286,7 +8412,9 @@
       <c r="T111" s="37"/>
     </row>
     <row r="112" spans="1:20" ht="18" customHeight="1">
-      <c r="A112" s="108"/>
+      <c r="A112" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B112" s="31" t="s">
         <v>132</v>
       </c>
@@ -8337,7 +8465,9 @@
       <c r="T112" s="37"/>
     </row>
     <row r="113" spans="1:20" ht="18" customHeight="1">
-      <c r="A113" s="108"/>
+      <c r="A113" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B113" s="31" t="s">
         <v>132</v>
       </c>
@@ -8388,7 +8518,9 @@
       <c r="T113" s="37"/>
     </row>
     <row r="114" spans="1:20" ht="18" customHeight="1">
-      <c r="A114" s="108"/>
+      <c r="A114" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B114" s="31" t="s">
         <v>132</v>
       </c>
@@ -8439,7 +8571,9 @@
       <c r="T114" s="37"/>
     </row>
     <row r="115" spans="1:20" ht="18" customHeight="1">
-      <c r="A115" s="108"/>
+      <c r="A115" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B115" s="31" t="s">
         <v>132</v>
       </c>
@@ -8490,7 +8624,9 @@
       <c r="T115" s="37"/>
     </row>
     <row r="116" spans="1:20" ht="18" customHeight="1">
-      <c r="A116" s="108"/>
+      <c r="A116" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B116" s="31" t="s">
         <v>132</v>
       </c>
@@ -8541,7 +8677,9 @@
       <c r="T116" s="37"/>
     </row>
     <row r="117" spans="1:20" ht="18" customHeight="1">
-      <c r="A117" s="49"/>
+      <c r="A117" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B117" s="31" t="s">
         <v>132</v>
       </c>
@@ -8590,7 +8728,9 @@
       <c r="T117" s="37"/>
     </row>
     <row r="118" spans="1:20" ht="18" customHeight="1">
-      <c r="A118" s="49"/>
+      <c r="A118" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B118" s="31" t="s">
         <v>132</v>
       </c>
@@ -8639,7 +8779,9 @@
       <c r="T118" s="37"/>
     </row>
     <row r="119" spans="1:20" ht="18" customHeight="1">
-      <c r="A119" s="49"/>
+      <c r="A119" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B119" s="31" t="s">
         <v>132</v>
       </c>
@@ -8688,7 +8830,9 @@
       <c r="T119" s="37"/>
     </row>
     <row r="120" spans="1:20" ht="18" customHeight="1">
-      <c r="A120" s="49"/>
+      <c r="A120" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B120" s="31" t="s">
         <v>132</v>
       </c>
@@ -8737,7 +8881,9 @@
       <c r="T120" s="37"/>
     </row>
     <row r="121" spans="1:20" ht="18" customHeight="1">
-      <c r="A121" s="49"/>
+      <c r="A121" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B121" s="31" t="s">
         <v>132</v>
       </c>
@@ -8786,7 +8932,9 @@
       <c r="T121" s="37"/>
     </row>
     <row r="122" spans="1:20" ht="18" customHeight="1">
-      <c r="A122" s="49"/>
+      <c r="A122" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B122" s="31" t="s">
         <v>132</v>
       </c>
@@ -8835,7 +8983,9 @@
       <c r="T122" s="37"/>
     </row>
     <row r="123" spans="1:20" ht="18" customHeight="1">
-      <c r="A123" s="49"/>
+      <c r="A123" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B123" s="31" t="s">
         <v>132</v>
       </c>
@@ -8884,7 +9034,9 @@
       <c r="T123" s="37"/>
     </row>
     <row r="124" spans="1:20" ht="18" customHeight="1">
-      <c r="A124" s="49"/>
+      <c r="A124" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B124" s="31" t="s">
         <v>132</v>
       </c>
@@ -8933,7 +9085,9 @@
       <c r="T124" s="37"/>
     </row>
     <row r="125" spans="1:20" ht="18" customHeight="1">
-      <c r="A125" s="49"/>
+      <c r="A125" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B125" s="31" t="s">
         <v>132</v>
       </c>
@@ -8982,7 +9136,9 @@
       <c r="T125" s="37"/>
     </row>
     <row r="126" spans="1:20" ht="18" customHeight="1">
-      <c r="A126" s="49"/>
+      <c r="A126" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B126" s="31" t="s">
         <v>132</v>
       </c>
@@ -9031,7 +9187,9 @@
       <c r="T126" s="37"/>
     </row>
     <row r="127" spans="1:20" ht="18" customHeight="1">
-      <c r="A127" s="49"/>
+      <c r="A127" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B127" s="31" t="s">
         <v>132</v>
       </c>
@@ -9080,7 +9238,9 @@
       <c r="T127" s="37"/>
     </row>
     <row r="128" spans="1:20" ht="18" customHeight="1">
-      <c r="A128" s="49"/>
+      <c r="A128" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B128" s="31" t="s">
         <v>132</v>
       </c>
@@ -9129,7 +9289,9 @@
       <c r="T128" s="37"/>
     </row>
     <row r="129" spans="1:20" ht="18" customHeight="1">
-      <c r="A129" s="49"/>
+      <c r="A129" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B129" s="31" t="s">
         <v>132</v>
       </c>
@@ -9178,7 +9340,9 @@
       <c r="T129" s="37"/>
     </row>
     <row r="130" spans="1:20" ht="18" customHeight="1">
-      <c r="A130" s="49"/>
+      <c r="A130" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B130" s="31" t="s">
         <v>132</v>
       </c>
@@ -9227,7 +9391,9 @@
       <c r="T130" s="37"/>
     </row>
     <row r="131" spans="1:20" ht="18" customHeight="1">
-      <c r="A131" s="49"/>
+      <c r="A131" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B131" s="31" t="s">
         <v>132</v>
       </c>
@@ -9276,7 +9442,9 @@
       <c r="T131" s="37"/>
     </row>
     <row r="132" spans="1:20" ht="18" customHeight="1">
-      <c r="A132" s="49"/>
+      <c r="A132" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B132" s="31" t="s">
         <v>132</v>
       </c>
@@ -9325,7 +9493,9 @@
       <c r="T132" s="37"/>
     </row>
     <row r="133" spans="1:20" ht="18" customHeight="1">
-      <c r="A133" s="49"/>
+      <c r="A133" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B133" s="31" t="s">
         <v>132</v>
       </c>
@@ -9376,7 +9546,9 @@
       <c r="T133" s="37"/>
     </row>
     <row r="134" spans="1:20" ht="18" customHeight="1">
-      <c r="A134" s="49"/>
+      <c r="A134" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B134" s="31" t="s">
         <v>132</v>
       </c>
@@ -9427,7 +9599,9 @@
       <c r="T134" s="37"/>
     </row>
     <row r="135" spans="1:20" ht="18" customHeight="1">
-      <c r="A135" s="49"/>
+      <c r="A135" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B135" s="31" t="s">
         <v>132</v>
       </c>
@@ -9478,7 +9652,9 @@
       <c r="T135" s="37"/>
     </row>
     <row r="136" spans="1:20" ht="18" customHeight="1">
-      <c r="A136" s="49"/>
+      <c r="A136" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B136" s="31" t="s">
         <v>132</v>
       </c>
@@ -9529,7 +9705,9 @@
       <c r="T136" s="37"/>
     </row>
     <row r="137" spans="1:20" ht="18" customHeight="1">
-      <c r="A137" s="49"/>
+      <c r="A137" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B137" s="31" t="s">
         <v>132</v>
       </c>
@@ -9580,7 +9758,9 @@
       <c r="T137" s="37"/>
     </row>
     <row r="138" spans="1:20" ht="18" customHeight="1">
-      <c r="A138" s="49"/>
+      <c r="A138" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B138" s="31" t="s">
         <v>132</v>
       </c>
@@ -9631,7 +9811,9 @@
       <c r="T138" s="37"/>
     </row>
     <row r="139" spans="1:20" ht="18" customHeight="1">
-      <c r="A139" s="49"/>
+      <c r="A139" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="B139" s="31" t="s">
         <v>132</v>
       </c>
@@ -9677,7 +9859,9 @@
       <c r="T139" s="37"/>
     </row>
     <row r="140" spans="1:20" ht="18" customHeight="1">
-      <c r="A140" s="49"/>
+      <c r="A140" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="B140" s="31" t="s">
         <v>132</v>
       </c>
@@ -9724,9 +9908,15 @@
     </row>
     <row r="141" spans="1:20" ht="18" customHeight="1">
       <c r="A141" s="49"/>
-      <c r="B141" s="31"/>
-      <c r="C141" s="90"/>
-      <c r="D141" s="30"/>
+      <c r="B141" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C141" s="90" t="s">
+        <v>153</v>
+      </c>
+      <c r="D141" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="E141" s="31"/>
       <c r="F141" s="32"/>
       <c r="G141" s="32"/>
@@ -9736,7 +9926,9 @@
       <c r="K141" s="35"/>
       <c r="L141" s="32"/>
       <c r="M141" s="32"/>
-      <c r="N141" s="30"/>
+      <c r="N141" s="36" t="s">
+        <v>155</v>
+      </c>
       <c r="O141" s="37"/>
       <c r="P141" s="38"/>
       <c r="Q141" s="38"/>
@@ -9746,9 +9938,15 @@
     </row>
     <row r="142" spans="1:20" ht="18" customHeight="1">
       <c r="A142" s="49"/>
-      <c r="B142" s="31"/>
-      <c r="C142" s="90"/>
-      <c r="D142" s="30"/>
+      <c r="B142" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="C142" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="D142" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="E142" s="31"/>
       <c r="F142" s="32"/>
       <c r="G142" s="32"/>
@@ -9758,7 +9956,9 @@
       <c r="K142" s="35"/>
       <c r="L142" s="32"/>
       <c r="M142" s="32"/>
-      <c r="N142" s="30"/>
+      <c r="N142" s="36" t="s">
+        <v>155</v>
+      </c>
       <c r="O142" s="37"/>
       <c r="P142" s="38"/>
       <c r="Q142" s="38"/>
@@ -9768,9 +9968,15 @@
     </row>
     <row r="143" spans="1:20" ht="18" customHeight="1">
       <c r="A143" s="49"/>
-      <c r="B143" s="31"/>
-      <c r="C143" s="30"/>
-      <c r="D143" s="30"/>
+      <c r="B143" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="C143" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D143" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="E143" s="31"/>
       <c r="F143" s="32"/>
       <c r="G143" s="32"/>
@@ -9780,7 +9986,9 @@
       <c r="K143" s="35"/>
       <c r="L143" s="32"/>
       <c r="M143" s="32"/>
-      <c r="N143" s="30"/>
+      <c r="N143" s="36" t="s">
+        <v>155</v>
+      </c>
       <c r="O143" s="37"/>
       <c r="P143" s="38"/>
       <c r="Q143" s="38"/>
@@ -9789,11 +9997,21 @@
       <c r="T143" s="37"/>
     </row>
     <row r="144" spans="1:20" ht="18" customHeight="1">
-      <c r="A144" s="49"/>
-      <c r="B144" s="31"/>
-      <c r="C144" s="90"/>
-      <c r="D144" s="30"/>
-      <c r="E144" s="31"/>
+      <c r="A144" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B144" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C144" s="90" t="s">
+        <v>153</v>
+      </c>
+      <c r="D144" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E144" s="31" t="s">
+        <v>154</v>
+      </c>
       <c r="F144" s="32"/>
       <c r="G144" s="32"/>
       <c r="H144" s="33"/>
@@ -9802,7 +10020,9 @@
       <c r="K144" s="35"/>
       <c r="L144" s="32"/>
       <c r="M144" s="32"/>
-      <c r="N144" s="30"/>
+      <c r="N144" s="36" t="s">
+        <v>155</v>
+      </c>
       <c r="O144" s="37"/>
       <c r="P144" s="38"/>
       <c r="Q144" s="38"/>
@@ -9812,44 +10032,100 @@
     </row>
     <row r="145" spans="1:20" ht="18" customHeight="1">
       <c r="A145" s="49"/>
-      <c r="B145" s="31"/>
-      <c r="C145" s="30"/>
-      <c r="D145" s="30"/>
+      <c r="B145" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="C145" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="D145" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="E145" s="31"/>
-      <c r="F145" s="32"/>
-      <c r="G145" s="32"/>
+      <c r="F145" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G145" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H145" s="33"/>
-      <c r="I145" s="34"/>
-      <c r="J145" s="35"/>
-      <c r="K145" s="35"/>
-      <c r="L145" s="32"/>
+      <c r="I145" s="34">
+        <v>298</v>
+      </c>
+      <c r="J145" s="35">
+        <f t="shared" ref="J145:K146" si="12">P145*9807000</f>
+        <v>4925075400</v>
+      </c>
+      <c r="K145" s="35">
+        <f t="shared" si="12"/>
+        <v>179468100</v>
+      </c>
+      <c r="L145" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M145" s="32"/>
-      <c r="N145" s="30"/>
+      <c r="N145" s="36" t="s">
+        <v>155</v>
+      </c>
       <c r="O145" s="37"/>
-      <c r="P145" s="38"/>
-      <c r="Q145" s="38"/>
+      <c r="P145" s="38">
+        <v>502.2</v>
+      </c>
+      <c r="Q145" s="38">
+        <v>18.3</v>
+      </c>
       <c r="R145" s="37"/>
       <c r="S145" s="37"/>
       <c r="T145" s="37"/>
     </row>
     <row r="146" spans="1:20" ht="18" customHeight="1">
-      <c r="A146" s="49"/>
-      <c r="B146" s="31"/>
-      <c r="C146" s="90"/>
-      <c r="D146" s="30"/>
-      <c r="E146" s="31"/>
-      <c r="F146" s="32"/>
-      <c r="G146" s="32"/>
+      <c r="A146" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B146" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C146" s="90" t="s">
+        <v>153</v>
+      </c>
+      <c r="D146" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E146" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F146" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G146" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H146" s="33"/>
-      <c r="I146" s="34"/>
-      <c r="J146" s="35"/>
-      <c r="K146" s="35"/>
-      <c r="L146" s="32"/>
+      <c r="I146" s="34">
+        <v>298</v>
+      </c>
+      <c r="J146" s="35">
+        <f t="shared" si="12"/>
+        <v>5866547400</v>
+      </c>
+      <c r="K146" s="35">
+        <f t="shared" si="12"/>
+        <v>240271500</v>
+      </c>
+      <c r="L146" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M146" s="32"/>
-      <c r="N146" s="30"/>
+      <c r="N146" s="36" t="s">
+        <v>155</v>
+      </c>
       <c r="O146" s="37"/>
-      <c r="P146" s="38"/>
-      <c r="Q146" s="38"/>
+      <c r="P146" s="38">
+        <v>598.20000000000005</v>
+      </c>
+      <c r="Q146" s="38">
+        <v>24.5</v>
+      </c>
       <c r="R146" s="37"/>
       <c r="S146" s="37"/>
       <c r="T146" s="37"/>
@@ -10449,7 +10725,7 @@
       <c r="T173" s="37"/>
     </row>
     <row r="174" spans="1:20" ht="18" customHeight="1">
-      <c r="A174" s="109"/>
+      <c r="A174" s="107"/>
       <c r="B174" s="102"/>
       <c r="C174" s="89"/>
       <c r="D174" s="89"/>
@@ -10457,7 +10733,7 @@
       <c r="F174" s="96"/>
       <c r="G174" s="96"/>
       <c r="H174" s="33"/>
-      <c r="I174" s="110"/>
+      <c r="I174" s="108"/>
       <c r="J174" s="47"/>
       <c r="K174" s="38"/>
       <c r="L174" s="32"/>
@@ -10471,7 +10747,7 @@
       <c r="T174" s="37"/>
     </row>
     <row r="175" spans="1:20" ht="18" customHeight="1">
-      <c r="A175" s="111"/>
+      <c r="A175" s="109"/>
       <c r="B175" s="104"/>
       <c r="C175" s="90"/>
       <c r="D175" s="90"/>
@@ -10479,7 +10755,7 @@
       <c r="F175" s="96"/>
       <c r="G175" s="97"/>
       <c r="H175" s="33"/>
-      <c r="I175" s="112"/>
+      <c r="I175" s="110"/>
       <c r="J175" s="47"/>
       <c r="K175" s="38"/>
       <c r="L175" s="32"/>
@@ -10493,7 +10769,7 @@
       <c r="T175" s="37"/>
     </row>
     <row r="176" spans="1:20" ht="18" customHeight="1">
-      <c r="A176" s="111"/>
+      <c r="A176" s="109"/>
       <c r="B176" s="104"/>
       <c r="C176" s="90"/>
       <c r="D176" s="90"/>
@@ -10501,7 +10777,7 @@
       <c r="F176" s="96"/>
       <c r="G176" s="97"/>
       <c r="H176" s="33"/>
-      <c r="I176" s="112"/>
+      <c r="I176" s="110"/>
       <c r="J176" s="47"/>
       <c r="K176" s="38"/>
       <c r="L176" s="32"/>
@@ -10515,7 +10791,7 @@
       <c r="T176" s="37"/>
     </row>
     <row r="177" spans="1:20" ht="18" customHeight="1">
-      <c r="A177" s="111"/>
+      <c r="A177" s="109"/>
       <c r="B177" s="104"/>
       <c r="C177" s="90"/>
       <c r="D177" s="90"/>
@@ -10523,7 +10799,7 @@
       <c r="F177" s="96"/>
       <c r="G177" s="97"/>
       <c r="H177" s="33"/>
-      <c r="I177" s="112"/>
+      <c r="I177" s="110"/>
       <c r="J177" s="35"/>
       <c r="K177" s="38"/>
       <c r="L177" s="32"/>
@@ -10537,7 +10813,7 @@
       <c r="T177" s="37"/>
     </row>
     <row r="178" spans="1:20" ht="18" customHeight="1">
-      <c r="A178" s="109"/>
+      <c r="A178" s="107"/>
       <c r="B178" s="102"/>
       <c r="C178" s="89"/>
       <c r="D178" s="89"/>
@@ -10545,7 +10821,7 @@
       <c r="F178" s="96"/>
       <c r="G178" s="96"/>
       <c r="H178" s="33"/>
-      <c r="I178" s="110"/>
+      <c r="I178" s="108"/>
       <c r="J178" s="35"/>
       <c r="K178" s="38"/>
       <c r="L178" s="32"/>
@@ -10559,7 +10835,7 @@
       <c r="T178" s="37"/>
     </row>
     <row r="179" spans="1:20" ht="18" customHeight="1">
-      <c r="A179" s="111"/>
+      <c r="A179" s="109"/>
       <c r="B179" s="104"/>
       <c r="C179" s="90"/>
       <c r="D179" s="90"/>
@@ -10567,7 +10843,7 @@
       <c r="F179" s="96"/>
       <c r="G179" s="97"/>
       <c r="H179" s="33"/>
-      <c r="I179" s="112"/>
+      <c r="I179" s="110"/>
       <c r="J179" s="35"/>
       <c r="K179" s="38"/>
       <c r="L179" s="32"/>
@@ -10581,7 +10857,7 @@
       <c r="T179" s="37"/>
     </row>
     <row r="180" spans="1:20" ht="18" customHeight="1">
-      <c r="A180" s="111"/>
+      <c r="A180" s="109"/>
       <c r="B180" s="104"/>
       <c r="C180" s="90"/>
       <c r="D180" s="90"/>
@@ -10589,7 +10865,7 @@
       <c r="F180" s="96"/>
       <c r="G180" s="97"/>
       <c r="H180" s="33"/>
-      <c r="I180" s="112"/>
+      <c r="I180" s="110"/>
       <c r="J180" s="35"/>
       <c r="K180" s="38"/>
       <c r="L180" s="32"/>
@@ -10603,7 +10879,7 @@
       <c r="T180" s="37"/>
     </row>
     <row r="181" spans="1:20" ht="18" customHeight="1">
-      <c r="A181" s="111"/>
+      <c r="A181" s="109"/>
       <c r="B181" s="104"/>
       <c r="C181" s="90"/>
       <c r="D181" s="90"/>
@@ -10611,7 +10887,7 @@
       <c r="F181" s="96"/>
       <c r="G181" s="97"/>
       <c r="H181" s="33"/>
-      <c r="I181" s="112"/>
+      <c r="I181" s="110"/>
       <c r="J181" s="35"/>
       <c r="K181" s="38"/>
       <c r="L181" s="32"/>
@@ -10713,7 +10989,7 @@
       <c r="T185" s="37"/>
     </row>
     <row r="186" spans="1:20" ht="18" customHeight="1">
-      <c r="A186" s="109"/>
+      <c r="A186" s="107"/>
       <c r="B186" s="102"/>
       <c r="C186" s="89"/>
       <c r="D186" s="89"/>
@@ -10735,7 +11011,7 @@
       <c r="T186" s="37"/>
     </row>
     <row r="187" spans="1:20" ht="18" customHeight="1">
-      <c r="A187" s="111"/>
+      <c r="A187" s="109"/>
       <c r="B187" s="104"/>
       <c r="C187" s="90"/>
       <c r="D187" s="90"/>
@@ -10757,7 +11033,7 @@
       <c r="T187" s="37"/>
     </row>
     <row r="188" spans="1:20" ht="18" customHeight="1">
-      <c r="A188" s="111"/>
+      <c r="A188" s="109"/>
       <c r="B188" s="104"/>
       <c r="C188" s="90"/>
       <c r="D188" s="90"/>
@@ -10779,7 +11055,7 @@
       <c r="T188" s="37"/>
     </row>
     <row r="189" spans="1:20" ht="18" customHeight="1">
-      <c r="A189" s="111"/>
+      <c r="A189" s="109"/>
       <c r="B189" s="104"/>
       <c r="C189" s="90"/>
       <c r="D189" s="90"/>
@@ -10801,7 +11077,7 @@
       <c r="T189" s="37"/>
     </row>
     <row r="190" spans="1:20" ht="18" customHeight="1">
-      <c r="A190" s="109"/>
+      <c r="A190" s="107"/>
       <c r="B190" s="102"/>
       <c r="C190" s="89"/>
       <c r="D190" s="89"/>
@@ -10823,7 +11099,7 @@
       <c r="T190" s="37"/>
     </row>
     <row r="191" spans="1:20" ht="18" customHeight="1">
-      <c r="A191" s="111"/>
+      <c r="A191" s="109"/>
       <c r="B191" s="104"/>
       <c r="C191" s="90"/>
       <c r="D191" s="90"/>
@@ -10845,7 +11121,7 @@
       <c r="T191" s="37"/>
     </row>
     <row r="192" spans="1:20" ht="18" customHeight="1">
-      <c r="A192" s="111"/>
+      <c r="A192" s="109"/>
       <c r="B192" s="104"/>
       <c r="C192" s="90"/>
       <c r="D192" s="90"/>
@@ -10867,7 +11143,7 @@
       <c r="T192" s="37"/>
     </row>
     <row r="193" spans="1:20" ht="18" customHeight="1">
-      <c r="A193" s="111"/>
+      <c r="A193" s="109"/>
       <c r="B193" s="104"/>
       <c r="C193" s="90"/>
       <c r="D193" s="90"/>
@@ -11026,7 +11302,7 @@
       <c r="C200" s="30"/>
       <c r="D200" s="30"/>
       <c r="E200" s="31"/>
-      <c r="F200" s="113"/>
+      <c r="F200" s="111"/>
       <c r="G200" s="32"/>
       <c r="H200" s="55"/>
       <c r="I200" s="53"/>
@@ -11395,7 +11671,7 @@
       <c r="T216" s="37"/>
     </row>
     <row r="217" spans="1:20" ht="18" customHeight="1">
-      <c r="A217" s="114"/>
+      <c r="A217" s="112"/>
       <c r="B217" s="102"/>
       <c r="C217" s="89"/>
       <c r="D217" s="89"/>
@@ -11417,7 +11693,7 @@
       <c r="T217" s="37"/>
     </row>
     <row r="218" spans="1:20" ht="18" customHeight="1">
-      <c r="A218" s="115"/>
+      <c r="A218" s="113"/>
       <c r="B218" s="104"/>
       <c r="C218" s="90"/>
       <c r="D218" s="90"/>
@@ -11439,7 +11715,7 @@
       <c r="T218" s="37"/>
     </row>
     <row r="219" spans="1:20" ht="18" customHeight="1">
-      <c r="A219" s="115"/>
+      <c r="A219" s="113"/>
       <c r="B219" s="104"/>
       <c r="C219" s="90"/>
       <c r="D219" s="90"/>
@@ -11461,7 +11737,7 @@
       <c r="T219" s="37"/>
     </row>
     <row r="220" spans="1:20" ht="18" customHeight="1">
-      <c r="A220" s="115"/>
+      <c r="A220" s="113"/>
       <c r="B220" s="104"/>
       <c r="C220" s="90"/>
       <c r="D220" s="90"/>
@@ -11483,7 +11759,7 @@
       <c r="T220" s="37"/>
     </row>
     <row r="221" spans="1:20" ht="18" customHeight="1">
-      <c r="A221" s="115"/>
+      <c r="A221" s="113"/>
       <c r="B221" s="104"/>
       <c r="C221" s="90"/>
       <c r="D221" s="90"/>
@@ -11505,7 +11781,7 @@
       <c r="T221" s="37"/>
     </row>
     <row r="222" spans="1:20" ht="18" customHeight="1">
-      <c r="A222" s="115"/>
+      <c r="A222" s="113"/>
       <c r="B222" s="104"/>
       <c r="C222" s="90"/>
       <c r="D222" s="90"/>
@@ -11527,7 +11803,7 @@
       <c r="T222" s="37"/>
     </row>
     <row r="223" spans="1:20" ht="18" customHeight="1">
-      <c r="A223" s="115"/>
+      <c r="A223" s="113"/>
       <c r="B223" s="104"/>
       <c r="C223" s="90"/>
       <c r="D223" s="90"/>
@@ -11549,7 +11825,7 @@
       <c r="T223" s="37"/>
     </row>
     <row r="224" spans="1:20" ht="18" customHeight="1">
-      <c r="A224" s="115"/>
+      <c r="A224" s="113"/>
       <c r="B224" s="104"/>
       <c r="C224" s="90"/>
       <c r="D224" s="90"/>
@@ -11571,7 +11847,7 @@
       <c r="T224" s="37"/>
     </row>
     <row r="225" spans="1:20" ht="18" customHeight="1">
-      <c r="A225" s="114"/>
+      <c r="A225" s="112"/>
       <c r="B225" s="102"/>
       <c r="C225" s="89"/>
       <c r="D225" s="89"/>
@@ -11593,7 +11869,7 @@
       <c r="T225" s="37"/>
     </row>
     <row r="226" spans="1:20" ht="18" customHeight="1">
-      <c r="A226" s="115"/>
+      <c r="A226" s="113"/>
       <c r="B226" s="104"/>
       <c r="C226" s="90"/>
       <c r="D226" s="90"/>
@@ -11615,7 +11891,7 @@
       <c r="T226" s="37"/>
     </row>
     <row r="227" spans="1:20" ht="18" customHeight="1">
-      <c r="A227" s="115"/>
+      <c r="A227" s="113"/>
       <c r="B227" s="104"/>
       <c r="C227" s="90"/>
       <c r="D227" s="90"/>
@@ -11637,7 +11913,7 @@
       <c r="T227" s="37"/>
     </row>
     <row r="228" spans="1:20" ht="18" customHeight="1">
-      <c r="A228" s="115"/>
+      <c r="A228" s="113"/>
       <c r="B228" s="104"/>
       <c r="C228" s="90"/>
       <c r="D228" s="90"/>
@@ -11659,7 +11935,7 @@
       <c r="T228" s="37"/>
     </row>
     <row r="229" spans="1:20" ht="18" customHeight="1">
-      <c r="A229" s="115"/>
+      <c r="A229" s="113"/>
       <c r="B229" s="104"/>
       <c r="C229" s="90"/>
       <c r="D229" s="90"/>
@@ -11681,7 +11957,7 @@
       <c r="T229" s="37"/>
     </row>
     <row r="230" spans="1:20" ht="18" customHeight="1">
-      <c r="A230" s="115"/>
+      <c r="A230" s="113"/>
       <c r="B230" s="104"/>
       <c r="C230" s="90"/>
       <c r="D230" s="90"/>
@@ -11703,7 +11979,7 @@
       <c r="T230" s="37"/>
     </row>
     <row r="231" spans="1:20" ht="18" customHeight="1">
-      <c r="A231" s="115"/>
+      <c r="A231" s="113"/>
       <c r="B231" s="104"/>
       <c r="C231" s="90"/>
       <c r="D231" s="90"/>
@@ -11725,7 +12001,7 @@
       <c r="T231" s="37"/>
     </row>
     <row r="232" spans="1:20" ht="18" customHeight="1">
-      <c r="A232" s="115"/>
+      <c r="A232" s="113"/>
       <c r="B232" s="104"/>
       <c r="C232" s="90"/>
       <c r="D232" s="90"/>
@@ -11747,7 +12023,7 @@
       <c r="T232" s="37"/>
     </row>
     <row r="233" spans="1:20" ht="18" customHeight="1">
-      <c r="A233" s="114"/>
+      <c r="A233" s="112"/>
       <c r="B233" s="102"/>
       <c r="C233" s="89"/>
       <c r="D233" s="89"/>
@@ -11769,7 +12045,7 @@
       <c r="T233" s="37"/>
     </row>
     <row r="234" spans="1:20" ht="18" customHeight="1">
-      <c r="A234" s="115"/>
+      <c r="A234" s="113"/>
       <c r="B234" s="104"/>
       <c r="C234" s="90"/>
       <c r="D234" s="90"/>
@@ -11791,7 +12067,7 @@
       <c r="T234" s="37"/>
     </row>
     <row r="235" spans="1:20" ht="18" customHeight="1">
-      <c r="A235" s="115"/>
+      <c r="A235" s="113"/>
       <c r="B235" s="104"/>
       <c r="C235" s="90"/>
       <c r="D235" s="90"/>
@@ -11813,7 +12089,7 @@
       <c r="T235" s="37"/>
     </row>
     <row r="236" spans="1:20" ht="18" customHeight="1">
-      <c r="A236" s="115"/>
+      <c r="A236" s="113"/>
       <c r="B236" s="104"/>
       <c r="C236" s="90"/>
       <c r="D236" s="90"/>
@@ -11835,7 +12111,7 @@
       <c r="T236" s="37"/>
     </row>
     <row r="237" spans="1:20" ht="18" customHeight="1">
-      <c r="A237" s="115"/>
+      <c r="A237" s="113"/>
       <c r="B237" s="104"/>
       <c r="C237" s="90"/>
       <c r="D237" s="90"/>
@@ -11857,7 +12133,7 @@
       <c r="T237" s="37"/>
     </row>
     <row r="238" spans="1:20" ht="18" customHeight="1">
-      <c r="A238" s="115"/>
+      <c r="A238" s="113"/>
       <c r="B238" s="104"/>
       <c r="C238" s="90"/>
       <c r="D238" s="90"/>
@@ -11879,7 +12155,7 @@
       <c r="T238" s="37"/>
     </row>
     <row r="239" spans="1:20" ht="18" customHeight="1">
-      <c r="A239" s="115"/>
+      <c r="A239" s="113"/>
       <c r="B239" s="104"/>
       <c r="C239" s="90"/>
       <c r="D239" s="90"/>
@@ -11901,7 +12177,7 @@
       <c r="T239" s="37"/>
     </row>
     <row r="240" spans="1:20" ht="18" customHeight="1">
-      <c r="A240" s="115"/>
+      <c r="A240" s="113"/>
       <c r="B240" s="104"/>
       <c r="C240" s="90"/>
       <c r="D240" s="90"/>
@@ -11923,7 +12199,7 @@
       <c r="T240" s="37"/>
     </row>
     <row r="241" spans="1:20" ht="18" customHeight="1">
-      <c r="A241" s="114"/>
+      <c r="A241" s="112"/>
       <c r="B241" s="102"/>
       <c r="C241" s="89"/>
       <c r="D241" s="89"/>
@@ -11945,7 +12221,7 @@
       <c r="T241" s="37"/>
     </row>
     <row r="242" spans="1:20" ht="18" customHeight="1">
-      <c r="A242" s="115"/>
+      <c r="A242" s="113"/>
       <c r="B242" s="104"/>
       <c r="C242" s="90"/>
       <c r="D242" s="90"/>
@@ -11967,7 +12243,7 @@
       <c r="T242" s="37"/>
     </row>
     <row r="243" spans="1:20" ht="18" customHeight="1">
-      <c r="A243" s="115"/>
+      <c r="A243" s="113"/>
       <c r="B243" s="104"/>
       <c r="C243" s="90"/>
       <c r="D243" s="90"/>
@@ -11989,7 +12265,7 @@
       <c r="T243" s="37"/>
     </row>
     <row r="244" spans="1:20" ht="18" customHeight="1">
-      <c r="A244" s="115"/>
+      <c r="A244" s="113"/>
       <c r="B244" s="104"/>
       <c r="C244" s="90"/>
       <c r="D244" s="90"/>
@@ -12011,7 +12287,7 @@
       <c r="T244" s="37"/>
     </row>
     <row r="245" spans="1:20" ht="18" customHeight="1">
-      <c r="A245" s="115"/>
+      <c r="A245" s="113"/>
       <c r="B245" s="104"/>
       <c r="C245" s="90"/>
       <c r="D245" s="90"/>
@@ -12033,7 +12309,7 @@
       <c r="T245" s="37"/>
     </row>
     <row r="246" spans="1:20" ht="18" customHeight="1">
-      <c r="A246" s="115"/>
+      <c r="A246" s="113"/>
       <c r="B246" s="104"/>
       <c r="C246" s="90"/>
       <c r="D246" s="90"/>
@@ -12055,7 +12331,7 @@
       <c r="T246" s="37"/>
     </row>
     <row r="247" spans="1:20" ht="18" customHeight="1">
-      <c r="A247" s="115"/>
+      <c r="A247" s="113"/>
       <c r="B247" s="104"/>
       <c r="C247" s="90"/>
       <c r="D247" s="90"/>
@@ -12077,7 +12353,7 @@
       <c r="T247" s="43"/>
     </row>
     <row r="248" spans="1:20" ht="18" customHeight="1">
-      <c r="A248" s="115"/>
+      <c r="A248" s="113"/>
       <c r="B248" s="104"/>
       <c r="C248" s="90"/>
       <c r="D248" s="90"/>
@@ -12099,7 +12375,7 @@
       <c r="T248" s="43"/>
     </row>
     <row r="249" spans="1:20" ht="18" customHeight="1">
-      <c r="A249" s="114"/>
+      <c r="A249" s="112"/>
       <c r="B249" s="102"/>
       <c r="C249" s="89"/>
       <c r="D249" s="89"/>
@@ -12121,7 +12397,7 @@
       <c r="T249" s="43"/>
     </row>
     <row r="250" spans="1:20" ht="18" customHeight="1">
-      <c r="A250" s="115"/>
+      <c r="A250" s="113"/>
       <c r="B250" s="104"/>
       <c r="C250" s="90"/>
       <c r="D250" s="90"/>
@@ -12143,7 +12419,7 @@
       <c r="T250" s="37"/>
     </row>
     <row r="251" spans="1:20" ht="18" customHeight="1">
-      <c r="A251" s="115"/>
+      <c r="A251" s="113"/>
       <c r="B251" s="104"/>
       <c r="C251" s="90"/>
       <c r="D251" s="90"/>
@@ -12165,7 +12441,7 @@
       <c r="T251" s="37"/>
     </row>
     <row r="252" spans="1:20" ht="18" customHeight="1">
-      <c r="A252" s="115"/>
+      <c r="A252" s="113"/>
       <c r="B252" s="104"/>
       <c r="C252" s="90"/>
       <c r="D252" s="90"/>
@@ -12187,7 +12463,7 @@
       <c r="T252" s="37"/>
     </row>
     <row r="253" spans="1:20" ht="18" customHeight="1">
-      <c r="A253" s="115"/>
+      <c r="A253" s="113"/>
       <c r="B253" s="104"/>
       <c r="C253" s="90"/>
       <c r="D253" s="90"/>
@@ -12209,7 +12485,7 @@
       <c r="T253" s="37"/>
     </row>
     <row r="254" spans="1:20" ht="18" customHeight="1">
-      <c r="A254" s="115"/>
+      <c r="A254" s="113"/>
       <c r="B254" s="104"/>
       <c r="C254" s="90"/>
       <c r="D254" s="90"/>
@@ -12231,7 +12507,7 @@
       <c r="T254" s="37"/>
     </row>
     <row r="255" spans="1:20" ht="18" customHeight="1">
-      <c r="A255" s="115"/>
+      <c r="A255" s="113"/>
       <c r="B255" s="104"/>
       <c r="C255" s="90"/>
       <c r="D255" s="90"/>
@@ -12253,7 +12529,7 @@
       <c r="T255" s="37"/>
     </row>
     <row r="256" spans="1:20" ht="18" customHeight="1">
-      <c r="A256" s="115"/>
+      <c r="A256" s="113"/>
       <c r="B256" s="104"/>
       <c r="C256" s="90"/>
       <c r="D256" s="90"/>
@@ -12275,7 +12551,7 @@
       <c r="T256" s="37"/>
     </row>
     <row r="257" spans="1:20" ht="18" customHeight="1">
-      <c r="A257" s="114"/>
+      <c r="A257" s="112"/>
       <c r="B257" s="102"/>
       <c r="C257" s="89"/>
       <c r="D257" s="89"/>
@@ -12297,7 +12573,7 @@
       <c r="T257" s="37"/>
     </row>
     <row r="258" spans="1:20" ht="18" customHeight="1">
-      <c r="A258" s="115"/>
+      <c r="A258" s="113"/>
       <c r="B258" s="104"/>
       <c r="C258" s="90"/>
       <c r="D258" s="90"/>
@@ -12319,7 +12595,7 @@
       <c r="T258" s="37"/>
     </row>
     <row r="259" spans="1:20" ht="18" customHeight="1">
-      <c r="A259" s="115"/>
+      <c r="A259" s="113"/>
       <c r="B259" s="104"/>
       <c r="C259" s="90"/>
       <c r="D259" s="90"/>
@@ -12341,7 +12617,7 @@
       <c r="T259" s="37"/>
     </row>
     <row r="260" spans="1:20" ht="18" customHeight="1">
-      <c r="A260" s="115"/>
+      <c r="A260" s="113"/>
       <c r="B260" s="104"/>
       <c r="C260" s="90"/>
       <c r="D260" s="90"/>
@@ -12363,7 +12639,7 @@
       <c r="T260" s="37"/>
     </row>
     <row r="261" spans="1:20" ht="18" customHeight="1">
-      <c r="A261" s="115"/>
+      <c r="A261" s="113"/>
       <c r="B261" s="104"/>
       <c r="C261" s="90"/>
       <c r="D261" s="90"/>
@@ -12385,7 +12661,7 @@
       <c r="T261" s="37"/>
     </row>
     <row r="262" spans="1:20" ht="18" customHeight="1">
-      <c r="A262" s="115"/>
+      <c r="A262" s="113"/>
       <c r="B262" s="104"/>
       <c r="C262" s="90"/>
       <c r="D262" s="90"/>
@@ -12407,7 +12683,7 @@
       <c r="T262" s="37"/>
     </row>
     <row r="263" spans="1:20" ht="18" customHeight="1">
-      <c r="A263" s="115"/>
+      <c r="A263" s="113"/>
       <c r="B263" s="104"/>
       <c r="C263" s="90"/>
       <c r="D263" s="90"/>
@@ -12429,7 +12705,7 @@
       <c r="T263" s="37"/>
     </row>
     <row r="264" spans="1:20" ht="18" customHeight="1">
-      <c r="A264" s="115"/>
+      <c r="A264" s="113"/>
       <c r="B264" s="104"/>
       <c r="C264" s="90"/>
       <c r="D264" s="90"/>
@@ -12460,7 +12736,7 @@
       <c r="G265" s="32"/>
       <c r="H265" s="55"/>
       <c r="I265" s="53"/>
-      <c r="J265" s="116"/>
+      <c r="J265" s="114"/>
       <c r="K265" s="38"/>
       <c r="L265" s="40"/>
       <c r="M265" s="40"/>
@@ -12482,7 +12758,7 @@
       <c r="G266" s="32"/>
       <c r="H266" s="55"/>
       <c r="I266" s="53"/>
-      <c r="J266" s="116"/>
+      <c r="J266" s="114"/>
       <c r="K266" s="38"/>
       <c r="L266" s="40"/>
       <c r="M266" s="40"/>
@@ -12504,7 +12780,7 @@
       <c r="G267" s="32"/>
       <c r="H267" s="55"/>
       <c r="I267" s="53"/>
-      <c r="J267" s="116"/>
+      <c r="J267" s="114"/>
       <c r="K267" s="38"/>
       <c r="L267" s="40"/>
       <c r="M267" s="40"/>
@@ -12526,7 +12802,7 @@
       <c r="G268" s="32"/>
       <c r="H268" s="55"/>
       <c r="I268" s="53"/>
-      <c r="J268" s="116"/>
+      <c r="J268" s="114"/>
       <c r="K268" s="38"/>
       <c r="L268" s="40"/>
       <c r="M268" s="40"/>

</xml_diff>